<commit_message>
Added in the Samurai skills doc 3 new skils.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/8-Samurai/Documentation/SamuraiSkills.xlsx
+++ b/GameDesign/Class/8-Samurai/Documentation/SamuraiSkills.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Client\Desktop\My_Dev\BattleForVoxturia\GameDesign\Class\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Client\Desktop\My_Dev\BattleForVoxturia\GameDesign\Class\8-Samurai\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil1 (2)" sheetId="2" r:id="rId2"/>
-    <sheet name="Feuil1 (3)" sheetId="3" r:id="rId3"/>
+    <sheet name="1-Dō-Maru" sheetId="1" r:id="rId1"/>
+    <sheet name="2-Keikogi" sheetId="2" r:id="rId2"/>
+    <sheet name="3-Banner" sheetId="3" r:id="rId3"/>
     <sheet name="Feuil1 (4)" sheetId="4" r:id="rId4"/>
     <sheet name="Feuil1 (5)" sheetId="5" r:id="rId5"/>
     <sheet name="Feuil1 (6)" sheetId="6" r:id="rId6"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="48">
   <si>
     <t>[[AP: 0 ]]</t>
   </si>
@@ -90,6 +90,93 @@
   </si>
   <si>
     <t>[[Number of turns between two casts: -  ]]</t>
+  </si>
+  <si>
+    <t>Dō-Maru</t>
+  </si>
+  <si>
+    <t>Unbuff ''Keikogi'' effect.</t>
+  </si>
+  <si>
+    <t>Effect name: ''Dō-Maru''.</t>
+  </si>
+  <si>
+    <t>[[AP: 1 ]]</t>
+  </si>
+  <si>
+    <t>[[MP: 1 ]]</t>
+  </si>
+  <si>
+    <t>[[Range: 0 ]]</t>
+  </si>
+  <si>
+    <t>[[Modifiable range: No ]]</t>
+  </si>
+  <si>
+    <t>[[Number of casts per turn: 1 ]]</t>
+  </si>
+  <si>
+    <t>[[Area of effect: - Single cell]]</t>
+  </si>
+  <si>
+    <t>[[Reduce taken damage by 20%]] (2 turns)</t>
+  </si>
+  <si>
+    <t>[[Reduce AP by 1]] (2 turns)</t>
+  </si>
+  <si>
+    <t>[[Reduce MP by 1]] (2 turns)</t>
+  </si>
+  <si>
+    <t>Reduces damage taken, but reduce AP and MP.                              Can not be cast in the Dō-Maru effect.</t>
+  </si>
+  <si>
+    <t>Keikogi</t>
+  </si>
+  <si>
+    <t>Effect name: ''Keikogi''.</t>
+  </si>
+  <si>
+    <t>Unbuff ''Dō-Maru'' effect.</t>
+  </si>
+  <si>
+    <t>[[Increase taken damage by 20%]] (2 turns)</t>
+  </si>
+  <si>
+    <t>[[Boost AP by 1]] (2 turns)</t>
+  </si>
+  <si>
+    <t>[[Boost MP by 2]] (2 turns)</t>
+  </si>
+  <si>
+    <t>Increase AP and MP but increase damage taken.                                               Can not be cast in the Dō-Maru effect.</t>
+  </si>
+  <si>
+    <t>Banner</t>
+  </si>
+  <si>
+    <t>[[AP: 3 ]]</t>
+  </si>
+  <si>
+    <t>[[Range: 1 ]]</t>
+  </si>
+  <si>
+    <t>[[Number of turns between two casts: 3 ]]</t>
+  </si>
+  <si>
+    <t>Self and allies: [[Increase damage by 15%]] (While in the glyph)</t>
+  </si>
+  <si>
+    <t>Self and allies: [[Increase resistance by 15%]] (While in the glyph)</t>
+  </si>
+  <si>
+    <t>Summons a ''Banner'' [[10% summoner HP, 0 AP, 0 MP, -10% earth resistence, -30% fire resistence, 25% water resistence, 25% air resistence, 50% light resistence, 50% dark resistence]] (1 turn)</t>
+  </si>
+  <si>
+    <t>Summon a ''Banner'' temporarily to increase damage and resistance of the summoner and his allies.</t>
+  </si>
+  <si>
+    <t>[[Area of effect: - Circle of 2 cells radius]]</t>
   </si>
 </sst>
 </file>
@@ -155,7 +242,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -172,11 +259,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -199,6 +301,16 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -514,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,7 +649,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -546,182 +658,142 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
+      <c r="C5" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="C10" s="3"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="C12" s="3"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C14" s="3"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
+      <c r="C17" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="12" t="s">
+        <v>29</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
+      <c r="C19" s="12" t="s">
+        <v>30</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
+      <c r="C25" s="13" t="s">
+        <v>21</v>
       </c>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="C26" s="13" t="s">
+        <v>20</v>
+      </c>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -948,10 +1020,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D27"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -971,7 +1043,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -980,182 +1052,142 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
+      <c r="C5" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="C10" s="3"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="C12" s="3"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C14" s="3"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
+      <c r="C17" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="12" t="s">
+        <v>36</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
+      <c r="C19" s="12" t="s">
+        <v>37</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
+      <c r="C25" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="C26" s="13" t="s">
+        <v>34</v>
+      </c>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1165,10 +1197,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D26"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1188,7 +1220,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1197,182 +1229,133 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
+      <c r="C5" s="11" t="s">
+        <v>46</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="C10" s="3"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="C12" s="3"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C14" s="3"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" ht="78.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
+      <c r="C17" s="14" t="s">
+        <v>45</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="12" t="s">
+        <v>43</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
+      <c r="C19" s="12" t="s">
+        <v>44</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="C25" s="10"/>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="D26" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added in Samurai skills doc 3 new skills.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/8-Samurai/Documentation/SamuraiSkills.xlsx
+++ b/GameDesign/Class/8-Samurai/Documentation/SamuraiSkills.xlsx
@@ -9,15 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="1-Dō-Maru" sheetId="1" r:id="rId1"/>
     <sheet name="2-Keikogi" sheetId="2" r:id="rId2"/>
     <sheet name="3-Banner" sheetId="3" r:id="rId3"/>
-    <sheet name="Feuil1 (4)" sheetId="4" r:id="rId4"/>
-    <sheet name="Feuil1 (5)" sheetId="5" r:id="rId5"/>
-    <sheet name="Feuil1 (6)" sheetId="6" r:id="rId6"/>
+    <sheet name="4-Katana" sheetId="4" r:id="rId4"/>
+    <sheet name="5-Wakizashi" sheetId="5" r:id="rId5"/>
+    <sheet name="6-Bokken" sheetId="6" r:id="rId6"/>
     <sheet name="Feuil1 (7)" sheetId="7" r:id="rId7"/>
     <sheet name="Feuil1 (8)" sheetId="8" r:id="rId8"/>
     <sheet name="Feuil1 (9)" sheetId="9" r:id="rId9"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="80">
   <si>
     <t>[[AP: 0 ]]</t>
   </si>
@@ -177,6 +177,102 @@
   </si>
   <si>
     <t>[[Area of effect: - Circle of 2 cells radius]]</t>
+  </si>
+  <si>
+    <t>Katana</t>
+  </si>
+  <si>
+    <t>[[AP: 4 ]]</t>
+  </si>
+  <si>
+    <t>[[Number of casts per turn: 2 ]]</t>
+  </si>
+  <si>
+    <t>[[Number of cast per turn per target: 1 ]]</t>
+  </si>
+  <si>
+    <t>[[Max effect accumulation: 3 ]]</t>
+  </si>
+  <si>
+    <t>Effect name: ''Cut''.</t>
+  </si>
+  <si>
+    <t>Target: [[''Cut'' effect +1 lvl]] (2 turns)</t>
+  </si>
+  <si>
+    <t>[[Area of effect: - Single cell ]]</t>
+  </si>
+  <si>
+    <t>Inflicts Earth-type damage.                                                                  The damage are higher when the target as ''Cut'' effect.</t>
+  </si>
+  <si>
+    <t>Wakizashi</t>
+  </si>
+  <si>
+    <t>[Damage:  60-75 earth ]]</t>
+  </si>
+  <si>
+    <t>[[Increase ''Katana'' damage by (50% * target ''Cut'' lvl)]]                     (2 turns)</t>
+  </si>
+  <si>
+    <t>[[Number of turns between two casts: 2 ]]</t>
+  </si>
+  <si>
+    <t>[[Damage:  15-20 earth ]]</t>
+  </si>
+  <si>
+    <t>Target: [[Reduce resistance by 25%]] (2 turns)</t>
+  </si>
+  <si>
+    <t>Inflicts Earth-type damage and reduce resistance.</t>
+  </si>
+  <si>
+    <t>Bokken</t>
+  </si>
+  <si>
+    <t>[[AP: 2 ]]</t>
+  </si>
+  <si>
+    <t>[[Number of casts per turn: 5 ]]</t>
+  </si>
+  <si>
+    <t>[[Number of cast per turn per target: 3 ]]</t>
+  </si>
+  <si>
+    <t>[[Max effect accumulation: 10 ]]</t>
+  </si>
+  <si>
+    <t>Effect name: ''Bokken''.</t>
+  </si>
+  <si>
+    <t>If the caster is under ''Keikogi'' effect:</t>
+  </si>
+  <si>
+    <t>If the caster is not under ''Keikogi'' effect:</t>
+  </si>
+  <si>
+    <t>When effect reach lvl 10, all the stacked effect are set to 2 turns.</t>
+  </si>
+  <si>
+    <t>[[Area of effect: - Single cell ]] (Must target an entity)</t>
+  </si>
+  <si>
+    <t>Stealth Air-type health                                                                        OR                                                                                                 Inflicts Earth-type damage.                                                                                                                                                                    Increase melee damage.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Target: [[Damage: 15-20 earth]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Caster: [[''Bokken'' effect +1 lvl]] (2 turns)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Target: [[Damage:  15-20 air steal ]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Caster: [[''Bokken'' effect +2 lvl]] (2 turns) </t>
+  </si>
+  <si>
+    <t>Caster: [[Boost melee damage by 10%]] (2 turns)</t>
   </si>
 </sst>
 </file>
@@ -242,7 +338,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -274,11 +370,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -312,6 +445,17 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1023,7 +1167,7 @@
   <dimension ref="B2:D27"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1199,7 +1343,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -1365,10 +1509,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D28"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1388,7 +1532,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1397,43 +1541,41 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
+      <c r="C5" s="11" t="s">
+        <v>56</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -1444,91 +1586,83 @@
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>4</v>
+      <c r="C12" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="C13" s="3"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="C16" s="3"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
+      <c r="C17" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
+      <c r="C19" s="15" t="s">
+        <v>58</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
+      <c r="C20" s="17" t="s">
+        <v>59</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="20" t="s">
+        <v>54</v>
+      </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
+      <c r="C25" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="D25" s="1"/>
     </row>
@@ -1537,42 +1671,17 @@
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B27" s="1"/>
+      <c r="C27" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" s="1"/>
+    </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="D28" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1582,10 +1691,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D24"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1605,7 +1714,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1614,43 +1723,41 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
+      <c r="C5" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -1662,134 +1769,73 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="C13" s="3"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>18</v>
+        <v>61</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
+      <c r="C17" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="10"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1801,8 +1847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D33"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1822,7 +1868,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1831,138 +1877,138 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="78" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
+      <c r="C5" s="18" t="s">
+        <v>74</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="10" t="s">
+        <v>65</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
-        <v>0</v>
+      <c r="C8" s="10" t="s">
+        <v>41</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="C9" s="10"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
+      <c r="C10" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="10"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>4</v>
+      <c r="C12" s="10" t="s">
+        <v>68</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="C13" s="10"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
+      <c r="C14" s="10" t="s">
+        <v>66</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="10" t="s">
+        <v>67</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="C16" s="10"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
+      <c r="C17" s="10" t="s">
+        <v>73</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
+      <c r="C19" s="15" t="s">
+        <v>70</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
+      <c r="C20" s="19" t="s">
+        <v>77</v>
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="16" t="s">
+        <v>78</v>
+      </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
+      <c r="C22" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="19" t="s">
+        <v>75</v>
+      </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
+      <c r="C24" s="16" t="s">
+        <v>76</v>
       </c>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
       <c r="C25" s="3" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
       <c r="D25" s="1"/>
     </row>
@@ -1991,22 +2037,22 @@
     </row>
     <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
+      <c r="C31" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B32" s="1"/>
       <c r="C32" s="10" t="s">
-        <v>17</v>
+        <v>72</v>
       </c>
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="D33" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added in Samurai skills doc 4 new skills. Samurai skills doc completed.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/8-Samurai/Documentation/SamuraiSkills.xlsx
+++ b/GameDesign/Class/8-Samurai/Documentation/SamuraiSkills.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="2" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="1-Dō-Maru" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,10 @@
     <sheet name="4-Katana" sheetId="4" r:id="rId4"/>
     <sheet name="5-Wakizashi" sheetId="5" r:id="rId5"/>
     <sheet name="6-Bokken" sheetId="6" r:id="rId6"/>
-    <sheet name="Feuil1 (7)" sheetId="7" r:id="rId7"/>
-    <sheet name="Feuil1 (8)" sheetId="8" r:id="rId8"/>
-    <sheet name="Feuil1 (9)" sheetId="9" r:id="rId9"/>
-    <sheet name="Feuil1 (10)" sheetId="10" r:id="rId10"/>
+    <sheet name="7-Hara-Kiri" sheetId="7" r:id="rId7"/>
+    <sheet name="8-Yumi" sheetId="8" r:id="rId8"/>
+    <sheet name="9-Kiai" sheetId="9" r:id="rId9"/>
+    <sheet name="10-Jinsoku" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -33,65 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="80">
-  <si>
-    <t>[[AP: 0 ]]</t>
-  </si>
-  <si>
-    <t>[[MP: 0 ]]</t>
-  </si>
-  <si>
-    <t>[[Range: 0-0 ]]</t>
-  </si>
-  <si>
-    <t>[[Cast in straight line: - ]]</t>
-  </si>
-  <si>
-    <t>[[Modifiable range: - ]]</t>
-  </si>
-  <si>
-    <t>[[Number of casts per turn: - ]]</t>
-  </si>
-  <si>
-    <t>[[Number of cast per turn per target: - ]]</t>
-  </si>
-  <si>
-    <t>[[Max effect accumulation: - ]]</t>
-  </si>
-  <si>
-    <t>[[Line of sight: - ]]</t>
-  </si>
-  <si>
-    <t>[[Area of effect: - Stright line of 1 cell]]</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="94">
   <si>
     <t>Additional Info</t>
   </si>
   <si>
-    <t>[[Damage:  0-0 fire ]]</t>
-  </si>
-  <si>
-    <t>EX: [[Boost taken damage by 10%]] (2 turns)</t>
-  </si>
-  <si>
-    <t>SKILL DESCRIPTION</t>
-  </si>
-  <si>
-    <t>¨¨ ¨¨</t>
-  </si>
-  <si>
-    <t>SKILL NAME</t>
-  </si>
-  <si>
-    <t>Effect name: ''X''.</t>
-  </si>
-  <si>
-    <t>Unbuff ''X'' effect.</t>
-  </si>
-  <si>
-    <t>[[Number of turns between two casts: -  ]]</t>
-  </si>
-  <si>
     <t>Dō-Maru</t>
   </si>
   <si>
@@ -273,6 +219,102 @@
   </si>
   <si>
     <t>Caster: [[Boost melee damage by 10%]] (2 turns)</t>
+  </si>
+  <si>
+    <t>Hara-Kiri</t>
+  </si>
+  <si>
+    <t>[[AP: 6 ]]</t>
+  </si>
+  <si>
+    <t>[[MP: 3 ]]</t>
+  </si>
+  <si>
+    <t>[[Number of turns between two casts: 00 ]]</t>
+  </si>
+  <si>
+    <t>[[Area of effect: - All the map ]]</t>
+  </si>
+  <si>
+    <t>Effect name: ''Hara-Kiri''.</t>
+  </si>
+  <si>
+    <t>Enemies: [[Increase taken damage by 25%]] (1 turn)</t>
+  </si>
+  <si>
+    <t>Allies: [[Increase damage by 25%]] (2 turns)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caster: [[Set K/O]] </t>
+  </si>
+  <si>
+    <t>The caster die to boost all his allies and weaken all his enemies.   The caster can only do it when his HP are at 20% or less.</t>
+  </si>
+  <si>
+    <t>Yumi</t>
+  </si>
+  <si>
+    <t>[[Range: 3-6 ]]</t>
+  </si>
+  <si>
+    <t>[[Modifiable range: Yes ]]</t>
+  </si>
+  <si>
+    <t>[[Line of sight: Yes ]]</t>
+  </si>
+  <si>
+    <t>[[Cast in straight line: No ]]</t>
+  </si>
+  <si>
+    <t>[[Damage:  5-50 air ]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Caster: [[''Yumi'' effect +1 lvl]] (2 turns)</t>
+  </si>
+  <si>
+    <t>Effect name: ''Yumi''.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Caster: [[Boost ranged damage by 10%]] (8 turns)</t>
+  </si>
+  <si>
+    <t>Inflicts Air-type damage and Increase ranged damage.</t>
+  </si>
+  <si>
+    <t>Kiai</t>
+  </si>
+  <si>
+    <t>[[Area of effect: - Circle of 2 cells radius ]]</t>
+  </si>
+  <si>
+    <t>Enemies: [[Damage: 5-10 air ]]</t>
+  </si>
+  <si>
+    <t>Caster: [[Increase next skill damage by 30%]]</t>
+  </si>
+  <si>
+    <t>Allies:  [[Increase next skill damage by 20%]]</t>
+  </si>
+  <si>
+    <t>Effect name: ''Kiai''.</t>
+  </si>
+  <si>
+    <t>Inflicts Air-type damage and increase the damage of the next skill.</t>
+  </si>
+  <si>
+    <t>Jinsoku</t>
+  </si>
+  <si>
+    <t>[[Number of turns between two casts: 4 ]]</t>
+  </si>
+  <si>
+    <t>[[Increase MP by MP / 2 (rounded up)]] (1 turn)</t>
+  </si>
+  <si>
+    <t>Effect name: ''Jinsoku''.</t>
+  </si>
+  <si>
+    <t>Increase the caster speed.</t>
   </si>
 </sst>
 </file>
@@ -411,12 +453,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -428,9 +467,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -792,20 +828,20 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>19</v>
+      <c r="C3" s="7" t="s">
+        <v>1</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="11" t="s">
-        <v>31</v>
+      <c r="C5" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -816,58 +852,58 @@
     </row>
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="3" t="s">
-        <v>22</v>
+      <c r="C7" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
-        <v>23</v>
+      <c r="C8" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>24</v>
+      <c r="C9" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3"/>
+      <c r="C10" s="2"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3" t="s">
-        <v>25</v>
+      <c r="C11" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3"/>
+      <c r="C12" s="2"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>26</v>
+      <c r="C13" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3"/>
+      <c r="C14" s="2"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3" t="s">
-        <v>27</v>
+      <c r="C15" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -878,22 +914,22 @@
     </row>
     <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
-      <c r="C17" s="12" t="s">
-        <v>28</v>
+      <c r="C17" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
-      <c r="C18" s="12" t="s">
-        <v>29</v>
+      <c r="C18" s="10" t="s">
+        <v>11</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="12" t="s">
-        <v>30</v>
+      <c r="C19" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="D19" s="1"/>
     </row>
@@ -910,8 +946,8 @@
     </row>
     <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
-      <c r="C23" s="5" t="s">
-        <v>10</v>
+      <c r="C23" s="4" t="s">
+        <v>0</v>
       </c>
       <c r="D23" s="1"/>
     </row>
@@ -922,22 +958,22 @@
     </row>
     <row r="25" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
-      <c r="C25" s="13" t="s">
-        <v>21</v>
+      <c r="C25" s="11" t="s">
+        <v>3</v>
       </c>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B26" s="1"/>
-      <c r="C26" s="13" t="s">
-        <v>20</v>
+      <c r="C26" s="11" t="s">
+        <v>2</v>
       </c>
       <c r="D26" s="1"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="6"/>
+      <c r="D27" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -947,10 +983,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D23"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -969,192 +1005,124 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>15</v>
+      <c r="C3" s="7" t="s">
+        <v>89</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
+      <c r="C5" s="9" t="s">
+        <v>93</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
-        <v>0</v>
+      <c r="C8" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="C9" s="2"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
+      <c r="C10" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="2"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>4</v>
+      <c r="C12" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="C13" s="2"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
+      <c r="C14" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
+      <c r="C16" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
-      </c>
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
+      <c r="C20" s="4" t="s">
+        <v>0</v>
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
+      <c r="C22" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="D23" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1186,20 +1154,20 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>32</v>
+      <c r="C3" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="11" t="s">
-        <v>38</v>
+      <c r="C5" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1210,58 +1178,58 @@
     </row>
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="3" t="s">
-        <v>22</v>
+      <c r="C7" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
-        <v>23</v>
+      <c r="C8" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>24</v>
+      <c r="C9" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3"/>
+      <c r="C10" s="2"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3" t="s">
-        <v>25</v>
+      <c r="C11" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3"/>
+      <c r="C12" s="2"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>26</v>
+      <c r="C13" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3"/>
+      <c r="C14" s="2"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3" t="s">
-        <v>27</v>
+      <c r="C15" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -1272,22 +1240,22 @@
     </row>
     <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
-      <c r="C17" s="3" t="s">
-        <v>35</v>
+      <c r="C17" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
-      <c r="C18" s="12" t="s">
-        <v>36</v>
+      <c r="C18" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="12" t="s">
-        <v>37</v>
+      <c r="C19" s="10" t="s">
+        <v>19</v>
       </c>
       <c r="D19" s="1"/>
     </row>
@@ -1304,8 +1272,8 @@
     </row>
     <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
-      <c r="C23" s="5" t="s">
-        <v>10</v>
+      <c r="C23" s="4" t="s">
+        <v>0</v>
       </c>
       <c r="D23" s="1"/>
     </row>
@@ -1316,22 +1284,22 @@
     </row>
     <row r="25" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
-      <c r="C25" s="13" t="s">
-        <v>33</v>
+      <c r="C25" s="11" t="s">
+        <v>15</v>
       </c>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B26" s="1"/>
-      <c r="C26" s="13" t="s">
-        <v>34</v>
+      <c r="C26" s="11" t="s">
+        <v>16</v>
       </c>
       <c r="D26" s="1"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="6"/>
+      <c r="D27" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1344,7 +1312,7 @@
   <dimension ref="B2:D26"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1363,20 +1331,20 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>39</v>
+      <c r="C3" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="11" t="s">
-        <v>46</v>
+      <c r="C5" s="9" t="s">
+        <v>28</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1387,58 +1355,58 @@
     </row>
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="3" t="s">
-        <v>40</v>
+      <c r="C7" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
-        <v>23</v>
+      <c r="C8" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>41</v>
+      <c r="C9" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3"/>
+      <c r="C10" s="2"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3" t="s">
-        <v>25</v>
+      <c r="C11" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3"/>
+      <c r="C12" s="2"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>42</v>
+      <c r="C13" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3"/>
+      <c r="C14" s="2"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3" t="s">
-        <v>47</v>
+      <c r="C15" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -1449,22 +1417,22 @@
     </row>
     <row r="17" spans="2:4" ht="78.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
-      <c r="C17" s="14" t="s">
-        <v>45</v>
+      <c r="C17" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
-      <c r="C18" s="12" t="s">
-        <v>43</v>
+      <c r="C18" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="12" t="s">
-        <v>44</v>
+      <c r="C19" s="10" t="s">
+        <v>26</v>
       </c>
       <c r="D19" s="1"/>
     </row>
@@ -1481,8 +1449,8 @@
     </row>
     <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
-      <c r="C23" s="5" t="s">
-        <v>10</v>
+      <c r="C23" s="4" t="s">
+        <v>0</v>
       </c>
       <c r="D23" s="1"/>
     </row>
@@ -1493,13 +1461,13 @@
     </row>
     <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
-      <c r="C25" s="10"/>
+      <c r="C25" s="8"/>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="6"/>
+      <c r="D26" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1531,20 +1499,20 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>48</v>
+      <c r="C3" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="11" t="s">
-        <v>56</v>
+      <c r="C5" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1555,70 +1523,70 @@
     </row>
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="3" t="s">
-        <v>49</v>
+      <c r="C7" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
-        <v>41</v>
+      <c r="C8" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3"/>
+      <c r="C9" s="2"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>25</v>
+      <c r="C10" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="2"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="7" t="s">
-        <v>52</v>
+      <c r="C12" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3"/>
+      <c r="C13" s="2"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>50</v>
+      <c r="C14" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3" t="s">
-        <v>51</v>
+      <c r="C15" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3"/>
+      <c r="C16" s="2"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="3" t="s">
-        <v>55</v>
+      <c r="C17" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -1629,22 +1597,22 @@
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
-      <c r="C19" s="15" t="s">
-        <v>58</v>
+      <c r="C19" s="13" t="s">
+        <v>40</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
-      <c r="C20" s="17" t="s">
-        <v>59</v>
+      <c r="C20" s="15" t="s">
+        <v>41</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
-      <c r="C21" s="20" t="s">
-        <v>54</v>
+      <c r="C21" s="18" t="s">
+        <v>36</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -1661,8 +1629,8 @@
     </row>
     <row r="25" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
-      <c r="C25" s="5" t="s">
-        <v>10</v>
+      <c r="C25" s="4" t="s">
+        <v>0</v>
       </c>
       <c r="D25" s="1"/>
     </row>
@@ -1673,15 +1641,15 @@
     </row>
     <row r="27" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B27" s="1"/>
-      <c r="C27" s="10" t="s">
-        <v>53</v>
+      <c r="C27" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="D27" s="1"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="6"/>
+      <c r="D28" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1713,20 +1681,20 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>57</v>
+      <c r="C3" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="11" t="s">
-        <v>63</v>
+      <c r="C5" s="9" t="s">
+        <v>45</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1737,51 +1705,51 @@
     </row>
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="3" t="s">
-        <v>40</v>
+      <c r="C7" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
-        <v>41</v>
+      <c r="C8" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3"/>
+      <c r="C9" s="2"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>25</v>
+      <c r="C10" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="2"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>60</v>
+      <c r="C12" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3"/>
+      <c r="C13" s="2"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>55</v>
+      <c r="C14" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -1792,15 +1760,15 @@
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>61</v>
+      <c r="C16" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="3" t="s">
-        <v>62</v>
+      <c r="C17" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -1817,8 +1785,8 @@
     </row>
     <row r="21" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
-      <c r="C21" s="5" t="s">
-        <v>10</v>
+      <c r="C21" s="4" t="s">
+        <v>0</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -1829,13 +1797,13 @@
     </row>
     <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
-      <c r="C23" s="10"/>
+      <c r="C23" s="8"/>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="6"/>
+      <c r="D24" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1847,8 +1815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1867,20 +1835,20 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>64</v>
+      <c r="C3" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="2:4" ht="78" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="18" t="s">
-        <v>74</v>
+      <c r="C5" s="16" t="s">
+        <v>56</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1891,70 +1859,70 @@
     </row>
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="10" t="s">
-        <v>65</v>
+      <c r="C7" s="8" t="s">
+        <v>47</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
-      <c r="C8" s="10" t="s">
-        <v>41</v>
+      <c r="C8" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="10"/>
+      <c r="C9" s="8"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="10" t="s">
-        <v>25</v>
+      <c r="C10" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="10"/>
+      <c r="C11" s="8"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="10" t="s">
-        <v>68</v>
+      <c r="C12" s="8" t="s">
+        <v>50</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="10"/>
+      <c r="C13" s="8"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="10" t="s">
-        <v>66</v>
+      <c r="C14" s="8" t="s">
+        <v>48</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="10" t="s">
-        <v>67</v>
+      <c r="C15" s="8" t="s">
+        <v>49</v>
       </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="10"/>
+      <c r="C16" s="8"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="10" t="s">
-        <v>73</v>
+      <c r="C17" s="8" t="s">
+        <v>55</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -1965,50 +1933,50 @@
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
-      <c r="C19" s="15" t="s">
-        <v>70</v>
+      <c r="C19" s="13" t="s">
+        <v>52</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
-      <c r="C20" s="19" t="s">
-        <v>77</v>
+      <c r="C20" s="17" t="s">
+        <v>59</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
-      <c r="C21" s="16" t="s">
-        <v>78</v>
+      <c r="C21" s="14" t="s">
+        <v>60</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
-      <c r="C22" s="15" t="s">
-        <v>71</v>
+      <c r="C22" s="13" t="s">
+        <v>53</v>
       </c>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
-      <c r="C23" s="19" t="s">
-        <v>75</v>
+      <c r="C23" s="17" t="s">
+        <v>57</v>
       </c>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
-      <c r="C24" s="16" t="s">
-        <v>76</v>
+      <c r="C24" s="14" t="s">
+        <v>58</v>
       </c>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>79</v>
+      <c r="C25" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="D25" s="1"/>
     </row>
@@ -2025,8 +1993,8 @@
     </row>
     <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
+      <c r="C29" s="4" t="s">
+        <v>0</v>
       </c>
       <c r="D29" s="1"/>
     </row>
@@ -2037,22 +2005,22 @@
     </row>
     <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B31" s="1"/>
-      <c r="C31" s="3" t="s">
-        <v>69</v>
+      <c r="C31" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="D31" s="1"/>
     </row>
     <row r="32" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>72</v>
+      <c r="C32" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="D32" s="1"/>
     </row>
     <row r="33" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="21"/>
+      <c r="D33" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2062,10 +2030,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D26"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2084,192 +2052,145 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>15</v>
+      <c r="C3" s="7" t="s">
+        <v>62</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
+      <c r="C5" s="9" t="s">
+        <v>71</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
-        <v>0</v>
+      <c r="C8" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>1</v>
+      <c r="C9" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="C10" s="2"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="C12" s="2"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>8</v>
+      <c r="C13" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C14" s="2"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
+      <c r="C17" s="10" t="s">
+        <v>70</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="10" t="s">
+        <v>69</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
+      <c r="C19" s="10" t="s">
+        <v>68</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="4" t="s">
+        <v>0</v>
+      </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
+      <c r="C25" s="8" t="s">
+        <v>67</v>
       </c>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="D26" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2279,10 +2200,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D32"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2301,148 +2222,148 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>15</v>
+      <c r="C3" s="7" t="s">
+        <v>72</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
+      <c r="C5" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
-        <v>0</v>
+      <c r="C8" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>1</v>
+      <c r="C9" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="C10" s="2"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>4</v>
+      <c r="C12" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>8</v>
+      <c r="C13" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C14" s="2"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="C16" s="2"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
+      <c r="C17" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C19" s="2"/>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
+      <c r="C20" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
+      <c r="C22" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="13" t="s">
+        <v>52</v>
+      </c>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
+      <c r="C24" s="17" t="s">
+        <v>78</v>
       </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
+      <c r="C25" s="14" t="s">
+        <v>80</v>
       </c>
       <c r="D25" s="1"/>
     </row>
@@ -2459,8 +2380,8 @@
     </row>
     <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
+      <c r="C29" s="4" t="s">
+        <v>0</v>
       </c>
       <c r="D29" s="1"/>
     </row>
@@ -2471,22 +2392,15 @@
     </row>
     <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
+      <c r="C31" s="8" t="s">
+        <v>79</v>
       </c>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2496,10 +2410,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D25"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2518,129 +2432,119 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>15</v>
+      <c r="C3" s="7" t="s">
+        <v>82</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
+      <c r="C5" s="9" t="s">
+        <v>88</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
-        <v>0</v>
+      <c r="C8" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="C9" s="2"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
+      <c r="C10" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="2"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>4</v>
+      <c r="C12" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="C13" s="2"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
+      <c r="C14" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
+      <c r="C16" s="10" t="s">
+        <v>84</v>
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
+      <c r="C17" s="10" t="s">
+        <v>85</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="10" t="s">
+        <v>86</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
+      <c r="C22" s="4" t="s">
+        <v>0</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -2651,59 +2555,15 @@
     </row>
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
+      <c r="C24" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>